<commit_message>
Añade lógica para validar corequisitos al cursar materias y mejora los mensajes de advertencia en la interfaz gráfica.
</commit_message>
<xml_diff>
--- a/Data/Pensum Enfermeria.xlsx
+++ b/Data/Pensum Enfermeria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\Desktop\App Pensum\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB533946-A0CD-466B-8C60-E82B938C6FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A7AC4C-15B8-4720-9C25-DF21C4034A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="825" windowWidth="21600" windowHeight="11295" xr2:uid="{794444EE-5232-4D64-AFA6-A9964823F49A}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{794444EE-5232-4D64-AFA6-A9964823F49A}"/>
   </bookViews>
   <sheets>
     <sheet name="Pensum" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="68">
   <si>
     <t>Código</t>
   </si>
@@ -62,17 +62,193 @@
     <t>Estado</t>
   </si>
   <si>
-    <t>juan</t>
-  </si>
-  <si>
     <t>Pendiente</t>
+  </si>
+  <si>
+    <t>BIOLOGÍA GENERAL</t>
+  </si>
+  <si>
+    <t>BIOQUÍMICA CLÍNICA</t>
+  </si>
+  <si>
+    <t>CÁTEDRA FARIA</t>
+  </si>
+  <si>
+    <t>EDUCACIÓN AMBIENTAL</t>
+  </si>
+  <si>
+    <t>ÉTICA</t>
+  </si>
+  <si>
+    <t>HABILIDADES COMUNICATIVAS</t>
+  </si>
+  <si>
+    <t>LABORATORIO BIOLOGÍA GENERAL</t>
+  </si>
+  <si>
+    <t>BIOESTADÍSTICA</t>
+  </si>
+  <si>
+    <t>FISIOLOGÍA</t>
+  </si>
+  <si>
+    <t>MARCO CONCEPTUAL Y FILOSÓFICO DE ENFERMERÍA</t>
+  </si>
+  <si>
+    <t>MICROBIOLOGÍA CLÍNICA</t>
+  </si>
+  <si>
+    <t>MODELIZACIÓN DE ROLES EN ENFERMERÍA</t>
+  </si>
+  <si>
+    <t>MORFOLOGÍA</t>
+  </si>
+  <si>
+    <t>CALIDAD, GESTIÓN Y EVALUACIÓN DE PROYECTOS EN SALUD</t>
+  </si>
+  <si>
+    <t>CUIDADO DE ENFERMERÍA EN SALUD COMUNITARIA I</t>
+  </si>
+  <si>
+    <t>EPIDEMIOLOGÍA</t>
+  </si>
+  <si>
+    <t>PROCESO DE VALORACIÓN DE ENFERMERIA</t>
+  </si>
+  <si>
+    <t>PROCESO DIAGNOSTICO DE ENFERMERÍA</t>
+  </si>
+  <si>
+    <t>BIENESTAR MENTAL</t>
+  </si>
+  <si>
+    <t>CUIDADO DE ENFERMERÍA EN SALUD COMUNITARIA II</t>
+  </si>
+  <si>
+    <t>ELECTIVA SOCIOHUMANÍSTICA I</t>
+  </si>
+  <si>
+    <t>FARMACOLOGÍA</t>
+  </si>
+  <si>
+    <t>LEGISLACIÓN EN ENFERMERÍA</t>
+  </si>
+  <si>
+    <t>CUIDADOS BÁSICOS DE ENFERMERÍA</t>
+  </si>
+  <si>
+    <t>ELECTIVA SOCIOHUMANÍSTICA II</t>
+  </si>
+  <si>
+    <t>EMPRESARISMO EN SALUD</t>
+  </si>
+  <si>
+    <t>GESTIÓN EN SERVICIOS DE SALUD</t>
+  </si>
+  <si>
+    <t>PSICOPATOLOGÍA Y PSIQUIATRÍA</t>
+  </si>
+  <si>
+    <t>CUIDADO DE ENFERMERÍA EN EL ADULTO</t>
+  </si>
+  <si>
+    <t>ELECTIVA DE PROFUNDIZACIÓN I</t>
+  </si>
+  <si>
+    <t>EMPRESAS DE CUIDADO EN ENFERMERÍA</t>
+  </si>
+  <si>
+    <t>SEMINARIO DE INVESTIGACIÓN EN SALUD</t>
+  </si>
+  <si>
+    <t>CUIDADO DE ENFERMERÍA EN EL ADULTO MAYOR</t>
+  </si>
+  <si>
+    <t>CUIDADO DE ENFERMERÍA EN EL NIÑO Y ADOLESCENTE</t>
+  </si>
+  <si>
+    <t>INVESTIGACIÓN EN SALUD</t>
+  </si>
+  <si>
+    <t>SALUD SEXUAL Y REPRODUCTIVA</t>
+  </si>
+  <si>
+    <t>CUIDADO DE ENFERMERÍA EN LA GESTANTE Y EL NEONATO</t>
+  </si>
+  <si>
+    <t>GERENCIA Y GESTIÓN EN EL CUIDADO DE ENFERMERÍA</t>
+  </si>
+  <si>
+    <t>INVESTIGACIÓN APLICADA EN SALUD</t>
+  </si>
+  <si>
+    <t>CAMPOS DE ACCIÓN PROFESIONAL CAP</t>
+  </si>
+  <si>
+    <t>ACTIV DEPOR.RECRE Y CULT-DEP UNIVERSITARIQ(EXTRAP)</t>
+  </si>
+  <si>
+    <t>CIVICA Y CONSTITUCION (EXTRAPLAN)</t>
+  </si>
+  <si>
+    <t>INFORMÁTICA BÁSICA (EXTRAPLAN)</t>
+  </si>
+  <si>
+    <t>156001/156005</t>
+  </si>
+  <si>
+    <t>162003/164010</t>
+  </si>
+  <si>
+    <t>172212/172213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+170001/170102/170103</t>
+  </si>
+  <si>
+    <t>172214/172215</t>
+  </si>
+  <si>
+    <t>172102/172207/172214/172215</t>
+  </si>
+  <si>
+    <t>170211/172208/172211</t>
+  </si>
+  <si>
+    <t>INTRODUCCIÓN A LA INVESTIGACIÓN 
+EN SALUD</t>
+  </si>
+  <si>
+    <t>172101/172214</t>
+  </si>
+  <si>
+    <t>153018/172202</t>
+  </si>
+  <si>
+    <t>172106/172209</t>
+  </si>
+  <si>
+    <t>159111/169101/174102</t>
+  </si>
+  <si>
+    <t>172205/172209</t>
+  </si>
+  <si>
+    <t>ELECTIVA DE PROFUNDIZACIÓN II</t>
+  </si>
+  <si>
+    <t>ELECTIVA DE PROFUNDIZACIÓN III</t>
+  </si>
+  <si>
+    <t>172104/172205/172209</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,7 +258,14 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -124,10 +307,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -463,15 +650,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8EDE00-C28F-473A-913C-A3B308A401C2}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="48" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,21 +695,1080 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A2" s="3">
+        <v>156001</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
+      <c r="D2" s="3">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A3" s="3">
+        <v>170101</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="D3" s="3">
+        <v>4</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A4" s="3">
+        <v>153002</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A5" s="3">
+        <v>164004</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A6" s="3">
+        <v>164010</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A7" s="3">
+        <v>162003</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A8" s="3">
+        <v>156005</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A9" s="3">
+        <v>157004</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A10" s="3">
+        <v>170102</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="48" x14ac:dyDescent="0.4">
+      <c r="A11" s="3">
+        <v>172212</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>3</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A12" s="3">
+        <v>170103</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>4</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="48" x14ac:dyDescent="0.4">
+      <c r="A13" s="3">
+        <v>172213</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3">
+        <v>3</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A14" s="3">
+        <v>170001</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3">
+        <v>3</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="48" x14ac:dyDescent="0.4">
+      <c r="A15" s="3">
+        <v>172102</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="3">
+        <v>3</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="48" x14ac:dyDescent="0.4">
+      <c r="A16" s="3">
+        <v>172207</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="3">
+        <v>3</v>
+      </c>
+      <c r="D16" s="3">
+        <v>5</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="3">
+        <v>172215</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A17" s="3">
+        <v>172103</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="3">
+        <v>3</v>
+      </c>
+      <c r="D17" s="3">
+        <v>4</v>
+      </c>
+      <c r="E17" s="3">
+        <v>157004</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="72" x14ac:dyDescent="0.4">
+      <c r="A18" s="3">
+        <v>172215</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="3">
+        <v>3</v>
+      </c>
+      <c r="D18" s="3">
+        <v>5</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="48" x14ac:dyDescent="0.4">
+      <c r="A19" s="3">
+        <v>172214</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="3">
+        <v>3</v>
+      </c>
+      <c r="D19" s="3">
+        <v>4</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="3">
+        <v>172215</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A20" s="3">
+        <v>172101</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="3">
+        <v>4</v>
+      </c>
+      <c r="D20" s="3">
+        <v>2</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3">
+        <v>0</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="48" x14ac:dyDescent="0.4">
+      <c r="A21" s="3">
+        <v>172208</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="3">
+        <v>4</v>
+      </c>
+      <c r="D21" s="3">
+        <v>6</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3">
+        <v>0</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A22" s="3">
+        <v>150001</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="3">
+        <v>4</v>
+      </c>
+      <c r="D22" s="3">
+        <v>2</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3">
+        <v>0</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A23" s="3">
+        <v>170211</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="3">
+        <v>4</v>
+      </c>
+      <c r="D23" s="3">
+        <v>5</v>
+      </c>
+      <c r="E23" s="3">
+        <v>170101</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3">
+        <v>0</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A24" s="3">
+        <v>172211</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="3">
+        <v>4</v>
+      </c>
+      <c r="D24" s="3">
+        <v>2</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3">
+        <v>0</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="48" x14ac:dyDescent="0.4">
+      <c r="A25" s="3">
+        <v>172202</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="3">
+        <v>5</v>
+      </c>
+      <c r="D25" s="3">
+        <v>6</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3">
+        <v>0</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A26" s="3">
+        <v>150002</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="3">
+        <v>5</v>
+      </c>
+      <c r="D26" s="3">
+        <v>2</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3">
+        <v>0</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A27" s="3">
+        <v>159111</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="3">
+        <v>5</v>
+      </c>
+      <c r="D27" s="3">
+        <v>3</v>
+      </c>
+      <c r="E27" s="3">
+        <v>172102</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3">
+        <v>0</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A28" s="3">
+        <v>169101</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="3">
+        <v>5</v>
+      </c>
+      <c r="D28" s="3">
+        <v>2</v>
+      </c>
+      <c r="E28" s="3">
+        <v>172102</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="48" x14ac:dyDescent="0.4">
+      <c r="A29" s="3">
+        <v>174102</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="3">
+        <v>5</v>
+      </c>
+      <c r="D29" s="3">
+        <v>2</v>
+      </c>
+      <c r="E29" s="3">
+        <v>172103</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A30" s="2">
+        <v>153018</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="3">
+        <v>5</v>
+      </c>
+      <c r="D30" s="3">
+        <v>2</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3">
+        <v>0</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A31" s="3">
+        <v>172205</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="3">
+        <v>6</v>
+      </c>
+      <c r="D31" s="3">
+        <v>10</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A32" s="3">
+        <v>172206</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="3">
+        <v>6</v>
+      </c>
+      <c r="D32" s="3">
+        <v>2</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3">
+        <v>0</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="48" x14ac:dyDescent="0.4">
+      <c r="A33" s="3">
+        <v>172209</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="3">
+        <v>6</v>
+      </c>
+      <c r="D33" s="3">
+        <v>2</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F33" s="3">
+        <v>172205</v>
+      </c>
+      <c r="G33" s="3">
+        <v>0</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="48" x14ac:dyDescent="0.4">
+      <c r="A34" s="3">
+        <v>172106</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="3">
+        <v>6</v>
+      </c>
+      <c r="D34" s="3">
+        <v>2</v>
+      </c>
+      <c r="E34" s="3">
+        <v>174102</v>
+      </c>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3">
+        <v>0</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="48" x14ac:dyDescent="0.4">
+      <c r="A35" s="3">
+        <v>172203</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="3">
+        <v>7</v>
+      </c>
+      <c r="D35" s="3">
+        <v>4</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F35" s="3">
+        <v>172104</v>
+      </c>
+      <c r="G35" s="3">
+        <v>0</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="48" x14ac:dyDescent="0.4">
+      <c r="A36" s="3">
+        <v>172204</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="3">
+        <v>7</v>
+      </c>
+      <c r="D36" s="3">
+        <v>5</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3">
+        <v>0</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A37" s="3">
+        <v>172104</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="3">
+        <v>7</v>
+      </c>
+      <c r="D37" s="3">
+        <v>2</v>
+      </c>
+      <c r="E37" s="3">
+        <v>172106</v>
+      </c>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3">
+        <v>0</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A38" s="3">
+        <v>170206</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="3">
+        <v>7</v>
+      </c>
+      <c r="D38" s="3">
+        <v>2</v>
+      </c>
+      <c r="E38" s="3">
+        <v>170202</v>
+      </c>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3">
+        <v>0</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A39" s="3">
+        <v>172001</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="3">
+        <v>7</v>
+      </c>
+      <c r="D39" s="3">
+        <v>2</v>
+      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3">
+        <v>0</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="48" x14ac:dyDescent="0.4">
+      <c r="A40" s="3">
+        <v>172206</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="3">
+        <v>8</v>
+      </c>
+      <c r="D40" s="3">
+        <v>10</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3">
+        <v>0</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A41" s="3">
+        <v>170206</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" s="3">
+        <v>8</v>
+      </c>
+      <c r="D41" s="3">
+        <v>2</v>
+      </c>
+      <c r="E41" s="2">
+        <v>170206</v>
+      </c>
+      <c r="F41" s="3">
+        <v>172210</v>
+      </c>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+    </row>
+    <row r="42" spans="1:8" ht="48" x14ac:dyDescent="0.4">
+      <c r="A42" s="3">
+        <v>172210</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="3">
+        <v>8</v>
+      </c>
+      <c r="D42" s="3">
+        <v>2</v>
+      </c>
+      <c r="E42" s="3">
+        <v>172209</v>
+      </c>
+      <c r="F42" s="3">
+        <v>170209</v>
+      </c>
+      <c r="G42" s="3">
+        <v>0</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A43" s="3">
+        <v>174103</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="3">
+        <v>8</v>
+      </c>
+      <c r="D43" s="3">
+        <v>2</v>
+      </c>
+      <c r="E43" s="3">
+        <v>172104</v>
+      </c>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3">
+        <v>0</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A44" s="3">
+        <v>172201</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="3">
         <v>9</v>
+      </c>
+      <c r="D44" s="3">
+        <v>16</v>
+      </c>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3">
+        <v>0</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="48" x14ac:dyDescent="0.4">
+      <c r="A45" s="3">
+        <v>173238</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="3">
+        <v>10</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0</v>
+      </c>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3">
+        <v>0</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A46" s="3">
+        <v>368006</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" s="3">
+        <v>10</v>
+      </c>
+      <c r="D46" s="3">
+        <v>0</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3">
+        <v>0</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A47" s="3">
+        <v>167281</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="3">
+        <v>10</v>
+      </c>
+      <c r="D47" s="3">
+        <v>0</v>
+      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3">
+        <v>0</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>